<commit_message>
Number Format Error Fixed
</commit_message>
<xml_diff>
--- a/excel/excelOutputFile.xlsx
+++ b/excel/excelOutputFile.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="41">
   <si>
     <t>No.</t>
   </si>
@@ -40,46 +40,103 @@
     <t>1</t>
   </si>
   <si>
-    <t>Hyundai Elite i20</t>
-  </si>
-  <si>
-    <t>Rs. 4.56 Lakh - 7.32 Lakh</t>
+    <t>Honda CBR150R</t>
+  </si>
+  <si>
+    <t>₹ 1.70 Lakh*</t>
+  </si>
+  <si>
+    <t>July 2024</t>
   </si>
   <si>
     <t>2</t>
   </si>
   <si>
-    <t>Hyundai Grand i10</t>
-  </si>
-  <si>
-    <t>Rs. 3.81 Lakh - 6.13 Lakh</t>
+    <t>Honda Rebel 300</t>
+  </si>
+  <si>
+    <t>₹ 2.30 Lakh*</t>
   </si>
   <si>
     <t>3</t>
   </si>
   <si>
-    <t>Honda Amaze</t>
-  </si>
-  <si>
-    <t>Rs. 3.97 Lakh - 9.77 Lakh</t>
+    <t>Honda NX200</t>
+  </si>
+  <si>
+    <t>₹ 1.20 Lakh*</t>
+  </si>
+  <si>
+    <t>August 2024</t>
   </si>
   <si>
     <t>4</t>
   </si>
   <si>
-    <t>Maruti Alto K10</t>
-  </si>
-  <si>
-    <t>Rs. 2.19 Lakh - 3.54 Lakh</t>
+    <t>Honda Hornet</t>
+  </si>
+  <si>
+    <t>₹ 2.50 Lakh*</t>
   </si>
   <si>
     <t>5</t>
   </si>
   <si>
-    <t>Tata NEXON</t>
-  </si>
-  <si>
-    <t>Rs. 5.85 Lakh - 10.96 Lakh</t>
+    <t>Honda XRE 300</t>
+  </si>
+  <si>
+    <t>₹ 3.00 Lakh*</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>Honda CBR300R</t>
+  </si>
+  <si>
+    <t>₹ 2.00 - ₹ 2.30 Lakh*</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>Honda NT1100</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>Honda CRF300L</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>Honda CB350 Cafe Racer</t>
+  </si>
+  <si>
+    <t>₹ 2.20 - ₹ 2.30 Lakh*</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>Honda CRF300 Rally</t>
+  </si>
+  <si>
+    <t>₹ 3.50 Lakh*</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>Honda CRF190L</t>
+  </si>
+  <si>
+    <t>₹ 1.98 Lakh*</t>
+  </si>
+  <si>
+    <t>September 2024</t>
   </si>
 </sst>
 </file>
@@ -124,7 +181,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -144,6 +201,160 @@
         <v>3</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s" s="0">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s" s="0">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s" s="0">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="D5" t="s" s="0">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="C6" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="D6" t="s" s="0">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="C7" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="D7" t="s" s="0">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="B8" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="C8" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="D8" t="s" s="0">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="B9" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="C9" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="D9" t="s" s="0">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s" s="0">
+        <v>31</v>
+      </c>
+      <c r="B10" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="C10" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="D10" t="s" s="0">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="B11" t="s" s="0">
+        <v>35</v>
+      </c>
+      <c r="C11" t="s" s="0">
+        <v>36</v>
+      </c>
+      <c r="D11" t="s" s="0">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="B12" t="s" s="0">
+        <v>38</v>
+      </c>
+      <c r="C12" t="s" s="0">
+        <v>39</v>
+      </c>
+      <c r="D12" t="s" s="0">
+        <v>40</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -151,7 +362,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C6"/>
+  <dimension ref="B1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -163,61 +374,6 @@
       </c>
       <c r="C1" t="s" s="0">
         <v>5</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s" s="0">
-        <v>8</v>
-      </c>
-      <c r="C2" t="s" s="0">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s" s="0">
-        <v>10</v>
-      </c>
-      <c r="B3" t="s" s="0">
-        <v>11</v>
-      </c>
-      <c r="C3" t="s" s="0">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s" s="0">
-        <v>13</v>
-      </c>
-      <c r="B4" t="s" s="0">
-        <v>14</v>
-      </c>
-      <c r="C4" t="s" s="0">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s" s="0">
-        <v>16</v>
-      </c>
-      <c r="B5" t="s" s="0">
-        <v>17</v>
-      </c>
-      <c r="C5" t="s" s="0">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s" s="0">
-        <v>19</v>
-      </c>
-      <c r="B6" t="s" s="0">
-        <v>20</v>
-      </c>
-      <c r="C6" t="s" s="0">
-        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>